<commit_message>
sir + seir epidemics
find best parameters for sir and seir minimizing loss function for dengue, zika, chicunguya
</commit_message>
<xml_diff>
--- a/administrative/main.xlsx
+++ b/administrative/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\pandemic_modelling\administrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA451EB-674D-41E1-99CA-55ED467C03BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95C0AC4-DE5B-44CF-B98F-9EC02F1C8332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="literature review" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="204">
   <si>
     <t>Pandemics &amp; Diffussion Models</t>
   </si>
@@ -659,9 +659,6 @@
     <t>Zika</t>
   </si>
   <si>
-    <t>Chicungunya</t>
-  </si>
-  <si>
     <t>Epidemics Weekly Full</t>
   </si>
   <si>
@@ -669,6 +666,15 @@
   </si>
   <si>
     <t>GGM + Refinement</t>
+  </si>
+  <si>
+    <t>Chicunguya</t>
+  </si>
+  <si>
+    <t>GGM+Refinement</t>
+  </si>
+  <si>
+    <t>R2 Summary</t>
   </si>
 </sst>
 </file>
@@ -678,9 +684,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,6 +774,19 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -817,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -848,10 +867,16 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1828,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1CF100-492E-4601-94D9-DFEFC6926913}">
   <dimension ref="B1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2116,7 +2141,7 @@
         <v>136</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -2127,7 +2152,7 @@
         <v>138</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -2138,7 +2163,7 @@
         <v>139</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -2171,7 +2196,7 @@
         <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -2182,7 +2207,7 @@
         <v>142</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -2369,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2EA5AC-0586-4893-B88A-0F9AA6E9FD44}">
-  <dimension ref="B1:AJ46"/>
+  <dimension ref="B1:AZ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AF17" sqref="AF17"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2400,18 +2425,27 @@
     <col min="26" max="26" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="2" style="20" customWidth="1"/>
-    <col min="29" max="29" width="15.109375" style="1" customWidth="1"/>
-    <col min="30" max="32" width="8.88671875" style="1"/>
-    <col min="33" max="33" width="2" style="20" customWidth="1"/>
-    <col min="34" max="16384" width="8.88671875" style="1"/>
+    <col min="29" max="31" width="12.109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="2" style="20" customWidth="1"/>
+    <col min="33" max="35" width="12.109375" style="1" customWidth="1"/>
+    <col min="36" max="36" width="2" style="20" customWidth="1"/>
+    <col min="37" max="37" width="15.109375" style="1" customWidth="1"/>
+    <col min="38" max="40" width="8.88671875" style="1"/>
+    <col min="41" max="41" width="2" style="20" customWidth="1"/>
+    <col min="42" max="44" width="8.88671875" style="1"/>
+    <col min="45" max="45" width="2" style="20" customWidth="1"/>
+    <col min="46" max="46" width="11.88671875" style="1" customWidth="1"/>
+    <col min="47" max="50" width="8.88671875" style="1"/>
+    <col min="51" max="51" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:52" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>186</v>
       </c>
@@ -2431,13 +2465,22 @@
       <c r="W2" s="19"/>
       <c r="X2" s="19"/>
       <c r="AC2" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG2" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK2" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP2" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="AH2" s="19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AT2" s="19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>181</v>
       </c>
@@ -2456,13 +2499,22 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="AC4" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH4" s="13" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="AG4" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>166</v>
       </c>
@@ -2533,25 +2585,62 @@
         <v>195</v>
       </c>
       <c r="AD6" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE6" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AG6" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AH6" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="AI6" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL6" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AE6" s="9" t="s">
+      <c r="AM6" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="AF6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="AH6" s="9" t="s">
+      <c r="AP6" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="AI6" s="9" t="s">
+      <c r="AQ6" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="AJ6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AT6" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AU6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV6" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW6" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AX6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY6" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AZ6" s="9"/>
+    </row>
+    <row r="7" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>171</v>
       </c>
@@ -2626,28 +2715,69 @@
         <v>15681.4452</v>
       </c>
       <c r="AC7" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD7" s="12">
+        <v>0.94224399999999997</v>
+      </c>
+      <c r="AE7" s="14">
+        <v>4703.6260300000004</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH7" s="12">
+        <v>0.91781400000000002</v>
+      </c>
+      <c r="AI7" s="14">
+        <v>5610.9171020000003</v>
+      </c>
+      <c r="AK7" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AL7" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AE7" s="12">
+      <c r="AM7" s="12">
         <v>-0.25174930000000001</v>
       </c>
-      <c r="AF7" s="14">
+      <c r="AN7" s="14">
         <v>210875.2597</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AP7" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AI7" s="24">
+      <c r="AQ7" s="24">
         <v>0.99999979999999999</v>
       </c>
-      <c r="AJ7" s="26">
+      <c r="AR7" s="26">
         <v>91.979789999999994</v>
       </c>
-    </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AT7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AU7" s="14">
+        <f>+_xlfn.XLOOKUP($AT7,$AC$7:$AC$9,$AE$7:$AE$9)</f>
+        <v>22520.654823000001</v>
+      </c>
+      <c r="AV7" s="14">
+        <f>+_xlfn.XLOOKUP(AT7,$AG$7:$AG$9,$AI$7:$AI$9)</f>
+        <v>18974.986979000001</v>
+      </c>
+      <c r="AW7" s="14">
+        <f>+AN7</f>
+        <v>210875.2597</v>
+      </c>
+      <c r="AX7" s="14">
+        <f>+AN8</f>
+        <v>15764.5885</v>
+      </c>
+      <c r="AY7" s="14">
+        <f>+AR7</f>
+        <v>91.979789999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>172</v>
       </c>
@@ -2724,26 +2854,67 @@
       <c r="AC8" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AD8" s="6" t="s">
+      <c r="AD8" s="18">
+        <v>0.98572300000000002</v>
+      </c>
+      <c r="AE8" s="17">
+        <v>22520.654823000001</v>
+      </c>
+      <c r="AG8" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH8" s="18">
+        <v>0.98986499999999999</v>
+      </c>
+      <c r="AI8" s="17">
+        <v>18974.986979000001</v>
+      </c>
+      <c r="AK8" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AE8" s="18">
+      <c r="AM8" s="18">
         <v>0.99300429999999995</v>
       </c>
-      <c r="AF8" s="17">
+      <c r="AN8" s="17">
         <v>15764.5885</v>
       </c>
-      <c r="AH8" s="6" t="s">
+      <c r="AP8" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AI8" s="25">
+      <c r="AQ8" s="25">
         <v>0.99997420000000004</v>
       </c>
-      <c r="AJ8" s="27">
+      <c r="AR8" s="27">
         <v>99.435940000000002</v>
       </c>
-    </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AT8" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU8" s="17">
+        <f t="shared" ref="AU8:AU9" si="7">+_xlfn.XLOOKUP(AT8,$AC$7:$AC$9,$AE$7:$AE$9)</f>
+        <v>4703.6260300000004</v>
+      </c>
+      <c r="AV8" s="17">
+        <f t="shared" ref="AV8:AV9" si="8">+_xlfn.XLOOKUP(AT8,$AG$7:$AG$9,$AI$7:$AI$9)</f>
+        <v>5610.9171020000003</v>
+      </c>
+      <c r="AW8" s="17">
+        <f>+AN9</f>
+        <v>1100.5509999999999</v>
+      </c>
+      <c r="AX8" s="17">
+        <f>+AN10</f>
+        <v>756.05920000000003</v>
+      </c>
+      <c r="AY8" s="17">
+        <f t="shared" ref="AY8:AY9" si="9">+AR8</f>
+        <v>99.435940000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>173</v>
       </c>
@@ -2818,28 +2989,69 @@
         <v>169850.0097</v>
       </c>
       <c r="AC9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD9" s="12">
+        <v>0.98843700000000001</v>
+      </c>
+      <c r="AE9" s="14">
+        <v>2148.462321</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH9" s="12">
+        <v>0.70254799999999995</v>
+      </c>
+      <c r="AI9" s="14">
+        <v>10896.633938999999</v>
+      </c>
+      <c r="AK9" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AL9" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AM9" s="12">
         <v>0.99683809999999995</v>
       </c>
-      <c r="AF9" s="14">
+      <c r="AN9" s="14">
         <v>1100.5509999999999</v>
       </c>
-      <c r="AH9" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI9" s="24">
+      <c r="AP9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AQ9" s="24">
         <v>0.9999806</v>
       </c>
-      <c r="AJ9" s="26">
+      <c r="AR9" s="26">
         <v>88.003110000000007</v>
       </c>
-    </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AT9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU9" s="14">
+        <f t="shared" si="7"/>
+        <v>2148.462321</v>
+      </c>
+      <c r="AV9" s="14">
+        <f t="shared" si="8"/>
+        <v>10896.633938999999</v>
+      </c>
+      <c r="AW9" s="14">
+        <f>+AN11</f>
+        <v>1976.5089</v>
+      </c>
+      <c r="AX9" s="14">
+        <f>+AN12</f>
+        <v>902.76419999999996</v>
+      </c>
+      <c r="AY9" s="14">
+        <f t="shared" si="9"/>
+        <v>88.003110000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>191</v>
       </c>
@@ -2913,20 +3125,25 @@
         <f t="shared" si="6"/>
         <v>425.01549999999997</v>
       </c>
-      <c r="AC10" s="6" t="s">
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="14"/>
+      <c r="AG10" s="14"/>
+      <c r="AH10" s="14"/>
+      <c r="AI10" s="14"/>
+      <c r="AK10" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AD10" s="6" t="s">
+      <c r="AL10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AE10" s="18">
+      <c r="AM10" s="18">
         <v>0.9985077</v>
       </c>
-      <c r="AF10" s="17">
+      <c r="AN10" s="17">
         <v>756.05920000000003</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>175</v>
       </c>
@@ -3000,20 +3217,25 @@
         <f t="shared" si="6"/>
         <v>39575.911200000002</v>
       </c>
-      <c r="AC11" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="14"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="14"/>
+      <c r="AK11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL11" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AE11" s="12">
+      <c r="AM11" s="12">
         <v>0.99021340000000002</v>
       </c>
-      <c r="AF11" s="14">
+      <c r="AN11" s="14">
         <v>1976.5089</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>176</v>
       </c>
@@ -3087,20 +3309,28 @@
         <f t="shared" si="6"/>
         <v>16566.6181</v>
       </c>
-      <c r="AC12" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD12" s="6" t="s">
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="14"/>
+      <c r="AG12" s="14"/>
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="14"/>
+      <c r="AK12" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AE12" s="18">
+      <c r="AM12" s="18">
         <v>0.99795840000000002</v>
       </c>
-      <c r="AF12" s="17">
+      <c r="AN12" s="17">
         <v>902.76419999999996</v>
       </c>
-    </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AT12" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>177</v>
       </c>
@@ -3174,8 +3404,14 @@
         <f t="shared" si="6"/>
         <v>24061.312300000001</v>
       </c>
-    </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AG13" s="14"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="14"/>
+    </row>
+    <row r="14" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>178</v>
       </c>
@@ -3249,8 +3485,17 @@
         <f t="shared" si="6"/>
         <v>1157.9239</v>
       </c>
-    </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AT14" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>179</v>
       </c>
@@ -3324,8 +3569,14 @@
         <f t="shared" si="6"/>
         <v>55078.919900000001</v>
       </c>
-    </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
+      <c r="AG15" s="14"/>
+      <c r="AH15" s="14"/>
+      <c r="AI15" s="14"/>
+    </row>
+    <row r="16" spans="2:52" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>180</v>
       </c>
@@ -3399,8 +3650,82 @@
         <f t="shared" si="6"/>
         <v>55089.632700000002</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AG16" s="14"/>
+      <c r="AH16" s="14"/>
+      <c r="AI16" s="14"/>
+      <c r="AT16" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AU16" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV16" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW16" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AX16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY16" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="2:51" x14ac:dyDescent="0.3">
+      <c r="AT17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AU17" s="12">
+        <f>+_xlfn.XLOOKUP($AT17,$AC$7:$AC$9,$AD$7:$AD$9)</f>
+        <v>0.98572300000000002</v>
+      </c>
+      <c r="AV17" s="12">
+        <f>+_xlfn.XLOOKUP(AT17,$AG$7:$AG$9,$AH$7:$AH$9)</f>
+        <v>0.98986499999999999</v>
+      </c>
+      <c r="AW17" s="12">
+        <f>+AM7</f>
+        <v>-0.25174930000000001</v>
+      </c>
+      <c r="AX17" s="12">
+        <f>+AM8</f>
+        <v>0.99300429999999995</v>
+      </c>
+      <c r="AY17" s="12">
+        <f>+AQ7</f>
+        <v>0.99999979999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:51" x14ac:dyDescent="0.3">
+      <c r="AT18" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU18" s="18">
+        <f t="shared" ref="AU18:AU19" si="10">+_xlfn.XLOOKUP($AT18,$AC$7:$AC$9,$AD$7:$AD$9)</f>
+        <v>0.94224399999999997</v>
+      </c>
+      <c r="AV18" s="18">
+        <f t="shared" ref="AV18:AV19" si="11">+_xlfn.XLOOKUP(AT18,$AG$7:$AG$9,$AH$7:$AH$9)</f>
+        <v>0.91781400000000002</v>
+      </c>
+      <c r="AW18" s="18">
+        <f>+AM9</f>
+        <v>0.99683809999999995</v>
+      </c>
+      <c r="AX18" s="18">
+        <f>+AM10</f>
+        <v>0.9985077</v>
+      </c>
+      <c r="AY18" s="18">
+        <f t="shared" ref="AY18:AY19" si="12">+AQ8</f>
+        <v>0.99997420000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>183</v>
       </c>
@@ -3411,14 +3736,37 @@
       <c r="V19" s="22"/>
       <c r="W19" s="22"/>
       <c r="X19" s="22"/>
-    </row>
-    <row r="20" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="AT19" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU19" s="12">
+        <f t="shared" si="10"/>
+        <v>0.98843700000000001</v>
+      </c>
+      <c r="AV19" s="12">
+        <f t="shared" si="11"/>
+        <v>0.70254799999999995</v>
+      </c>
+      <c r="AW19" s="12">
+        <f>+AM11</f>
+        <v>0.99021340000000002</v>
+      </c>
+      <c r="AX19" s="12">
+        <f>+AM12</f>
+        <v>0.99795840000000002</v>
+      </c>
+      <c r="AY19" s="12">
+        <f t="shared" si="12"/>
+        <v>0.9999806</v>
+      </c>
+    </row>
+    <row r="20" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="T20" s="21"/>
       <c r="V20" s="23"/>
       <c r="W20" s="23"/>
       <c r="X20" s="23"/>
     </row>
-    <row r="21" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>166</v>
       </c>
@@ -3454,7 +3802,7 @@
       <c r="W21" s="23"/>
       <c r="X21" s="23"/>
     </row>
-    <row r="22" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>171</v>
       </c>
@@ -3492,7 +3840,7 @@
       <c r="W22" s="23"/>
       <c r="X22" s="23"/>
     </row>
-    <row r="23" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>172</v>
       </c>
@@ -3509,7 +3857,7 @@
         <v>191678.16</v>
       </c>
       <c r="G23" s="6" t="str">
-        <f t="shared" ref="G23:G31" si="7">+IF(F23&lt;D23,"GGM","BM")</f>
+        <f t="shared" ref="G23:G31" si="13">+IF(F23&lt;D23,"GGM","BM")</f>
         <v>GGM</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -3522,15 +3870,21 @@
         <v>7970.5929999999998</v>
       </c>
       <c r="L23" s="17">
-        <f t="shared" ref="L23:L31" si="8">+K23-_xlfn.XLOOKUP(I23,B$22:B$31,F$22:F$31)</f>
+        <f t="shared" ref="L23:L31" si="14">+K23-_xlfn.XLOOKUP(I23,B$22:B$31,F$22:F$31)</f>
         <v>-183707.56700000001</v>
       </c>
       <c r="T23" s="21"/>
       <c r="V23" s="23"/>
       <c r="W23" s="23"/>
       <c r="X23" s="23"/>
-    </row>
-    <row r="24" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="AC23" s="28"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="28"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
+      <c r="AI23" s="28"/>
+    </row>
+    <row r="24" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>173</v>
       </c>
@@ -3547,7 +3901,7 @@
         <v>170016.12</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -3560,15 +3914,21 @@
         <v>10259.941000000001</v>
       </c>
       <c r="L24" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-159756.179</v>
       </c>
       <c r="T24" s="21"/>
       <c r="V24" s="23"/>
       <c r="W24" s="23"/>
       <c r="X24" s="23"/>
-    </row>
-    <row r="25" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+    </row>
+    <row r="25" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>174</v>
       </c>
@@ -3585,7 +3945,7 @@
         <v>20254.93</v>
       </c>
       <c r="G25" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I25" s="6" t="s">
@@ -3598,15 +3958,21 @@
         <v>2682.71</v>
       </c>
       <c r="L25" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-17572.22</v>
       </c>
       <c r="T25" s="21"/>
       <c r="V25" s="23"/>
       <c r="W25" s="23"/>
       <c r="X25" s="23"/>
-    </row>
-    <row r="26" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="29"/>
+      <c r="AE25" s="29"/>
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="29"/>
+      <c r="AI25" s="29"/>
+    </row>
+    <row r="26" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>175</v>
       </c>
@@ -3623,7 +3989,7 @@
         <v>1270365.45</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -3636,15 +4002,21 @@
         <v>54571.813999999998</v>
       </c>
       <c r="L26" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-1215793.6359999999</v>
       </c>
       <c r="T26" s="21"/>
       <c r="V26" s="23"/>
       <c r="W26" s="23"/>
       <c r="X26" s="23"/>
-    </row>
-    <row r="27" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="29"/>
+      <c r="AI26" s="29"/>
+    </row>
+    <row r="27" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>176</v>
       </c>
@@ -3661,7 +4033,7 @@
         <v>962242.14</v>
       </c>
       <c r="G27" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -3674,7 +4046,7 @@
         <v>37554.368000000002</v>
       </c>
       <c r="L27" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-924687.772</v>
       </c>
       <c r="T27" s="21"/>
@@ -3682,7 +4054,7 @@
       <c r="W27" s="23"/>
       <c r="X27" s="23"/>
     </row>
-    <row r="28" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>177</v>
       </c>
@@ -3699,7 +4071,7 @@
         <v>177553.42</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -3712,7 +4084,7 @@
         <v>18001.951000000001</v>
       </c>
       <c r="L28" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-159551.46900000001</v>
       </c>
       <c r="T28" s="21"/>
@@ -3720,7 +4092,7 @@
       <c r="W28" s="23"/>
       <c r="X28" s="23"/>
     </row>
-    <row r="29" spans="2:24" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:51" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>178</v>
       </c>
@@ -3737,7 +4109,7 @@
         <v>41689.589999999997</v>
       </c>
       <c r="G29" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I29" s="6" t="s">
@@ -3750,7 +4122,7 @@
         <v>2688.72</v>
       </c>
       <c r="L29" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-39000.869999999995</v>
       </c>
       <c r="T29" s="21"/>
@@ -3758,7 +4130,7 @@
       <c r="W29" s="23"/>
       <c r="X29" s="23"/>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>179</v>
       </c>
@@ -3775,7 +4147,7 @@
         <v>55105.7</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -3788,11 +4160,11 @@
         <v>3653520.236</v>
       </c>
       <c r="L30" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-4.0000001899898052E-3</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:51" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>180</v>
       </c>
@@ -3809,7 +4181,7 @@
         <v>3653520.24</v>
       </c>
       <c r="G31" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>GGM</v>
       </c>
       <c r="I31" s="6" t="s">
@@ -3822,7 +4194,7 @@
         <v>2309.4769999999999</v>
       </c>
       <c r="L31" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-52796.222999999998</v>
       </c>
     </row>
@@ -3917,7 +4289,7 @@
         <v>211942.1</v>
       </c>
       <c r="G38" s="6" t="str">
-        <f t="shared" ref="G38:G46" si="9">+IF(F38&lt;D38,"GGM","BM")</f>
+        <f t="shared" ref="G38:G46" si="15">+IF(F38&lt;D38,"GGM","BM")</f>
         <v>GGM</v>
       </c>
       <c r="I38" s="6" t="s">
@@ -3930,7 +4302,7 @@
         <v>100789.75999999999</v>
       </c>
       <c r="L38" s="17">
-        <f t="shared" ref="L38:L46" si="10">+K38-_xlfn.XLOOKUP(I38,B$37:B$46,F$37:F$46)</f>
+        <f t="shared" ref="L38:L46" si="16">+K38-_xlfn.XLOOKUP(I38,B$37:B$46,F$37:F$46)</f>
         <v>-111152.34000000001</v>
       </c>
     </row>
@@ -3951,7 +4323,7 @@
         <v>174775.12</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -3964,7 +4336,7 @@
         <v>120410.38</v>
       </c>
       <c r="L39" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-54364.739999999991</v>
       </c>
     </row>
@@ -3985,7 +4357,7 @@
         <v>23030.65</v>
       </c>
       <c r="G40" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I40" s="6" t="s">
@@ -3998,7 +4370,7 @@
         <v>18214.75</v>
       </c>
       <c r="L40" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-4815.9000000000015</v>
       </c>
     </row>
@@ -4019,7 +4391,7 @@
         <v>1236195.68</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -4032,7 +4404,7 @@
         <v>510440.15</v>
       </c>
       <c r="L41" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-725755.52999999991</v>
       </c>
     </row>
@@ -4053,7 +4425,7 @@
         <v>1098061.48</v>
       </c>
       <c r="G42" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I42" s="6" t="s">
@@ -4066,7 +4438,7 @@
         <v>631028.31999999995</v>
       </c>
       <c r="L42" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-467033.16000000003</v>
       </c>
     </row>
@@ -4087,7 +4459,7 @@
         <v>198641.06</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -4100,7 +4472,7 @@
         <v>126978.78</v>
       </c>
       <c r="L43" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-71662.28</v>
       </c>
     </row>
@@ -4121,7 +4493,7 @@
         <v>46165.85</v>
       </c>
       <c r="G44" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I44" s="6" t="s">
@@ -4134,7 +4506,7 @@
         <v>29197.63</v>
       </c>
       <c r="L44" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-16968.219999999998</v>
       </c>
     </row>
@@ -4155,7 +4527,7 @@
         <v>53945.74</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -4168,7 +4540,7 @@
         <v>4077694.45</v>
       </c>
       <c r="L45" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -4189,7 +4561,7 @@
         <v>4077694.45</v>
       </c>
       <c r="G46" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>GGM</v>
       </c>
       <c r="I46" s="6" t="s">
@@ -4202,13 +4574,13 @@
         <v>30806.880000000001</v>
       </c>
       <c r="L46" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-23138.859999999997</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="W7:AA16">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="W7:AA16 AC13:AE16 AG13:AI16">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
add some info to main xlsx
</commit_message>
<xml_diff>
--- a/administrative/main.xlsx
+++ b/administrative/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\pandemic_modelling\administrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95C0AC4-DE5B-44CF-B98F-9EC02F1C8332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48584632-088B-4AB9-BDB4-836BE47FD4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="literature review" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="modelling" sheetId="6" r:id="rId5"/>
     <sheet name="results" sheetId="8" r:id="rId6"/>
     <sheet name="Ideas" sheetId="5" r:id="rId7"/>
-    <sheet name="help" sheetId="7" r:id="rId8"/>
+    <sheet name="pytrends_categories" sheetId="9" r:id="rId8"/>
+    <sheet name="help" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="226">
   <si>
     <t>Pandemics &amp; Diffussion Models</t>
   </si>
@@ -675,6 +676,72 @@
   </si>
   <si>
     <t>R2 Summary</t>
+  </si>
+  <si>
+    <t>Google trends health</t>
+  </si>
+  <si>
+    <t>Pytrends useful categories</t>
+  </si>
+  <si>
+    <t>Health News: 1253</t>
+  </si>
+  <si>
+    <t>Health Policy: 1256</t>
+  </si>
+  <si>
+    <t>Medical Facilities &amp; Services: 256</t>
+  </si>
+  <si>
+    <t>Public Health: 947</t>
+  </si>
+  <si>
+    <t>Health Conditions: 419</t>
+  </si>
+  <si>
+    <t>Health: 45</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/10.1177/14604582241275844?icid=int.sj-full-text.citing-articles.1</t>
+  </si>
+  <si>
+    <t>ML epidemics</t>
+  </si>
+  <si>
+    <t>AI-based epidemic and pandemic early warning systems: A systematic scoping review</t>
+  </si>
+  <si>
+    <t>temperature, humitiy</t>
+  </si>
+  <si>
+    <t>demographic density</t>
+  </si>
+  <si>
+    <t># healt facilities</t>
+  </si>
+  <si>
+    <t>uv radiation band, ask einer</t>
+  </si>
+  <si>
+    <t>altimetry</t>
+  </si>
+  <si>
+    <t>WASTEWATER</t>
+  </si>
+  <si>
+    <t>pharmacy sales</t>
+  </si>
+  <si>
+    <t>pharmacy google trends</t>
+  </si>
+  <si>
+    <t>animal health data</t>
+  </si>
+  <si>
+    <t>do hybrid GGM-ML / SIR-ML</t>
+  </si>
+  <si>
+    <t>Use alternative data (satelite, mobility, searches, nlp_</t>
   </si>
 </sst>
 </file>
@@ -836,7 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -877,6 +944,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1212,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354077A2-E602-4D9A-90DA-98AD5E623913}">
-  <dimension ref="B1:F24"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,6 +1607,20 @@
       </c>
       <c r="E24" s="4" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1565,6 +1647,7 @@
     <hyperlink ref="E22" r:id="rId20" xr:uid="{94F4A7D7-3F55-4643-9FD0-A11EF159A4C1}"/>
     <hyperlink ref="E23" r:id="rId21" xr:uid="{3D99AF48-A732-4ADA-B469-518D1E1C4F59}"/>
     <hyperlink ref="E24" r:id="rId22" xr:uid="{EAAB6CA0-E60C-4CCA-9A60-6D6314C9AA39}"/>
+    <hyperlink ref="E25" r:id="rId23" xr:uid="{4730B165-77B9-44CC-96F1-5D46B06A3B46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1853,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1CF100-492E-4601-94D9-DFEFC6926913}">
   <dimension ref="B1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4597,10 +4680,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE21AE24-7B23-4499-8D22-C9A70AD3E5F9}">
-  <dimension ref="B1:C26"/>
+  <dimension ref="B1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4808,12 +4891,132 @@
         <v>163</v>
       </c>
     </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCC3A30-8DEB-4A80-AC0D-2CC25A9FC432}">
+  <dimension ref="B1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5625718-4007-43A2-8FA5-6282944FC450}">
   <dimension ref="B1:B5"/>
   <sheetViews>

</xml_diff>